<commit_message>
bind và render cho định mức nhân công và máy
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -13,6 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Tiên lượng" sheetId="1" r:id="rId1"/>
+    <sheet name="Định mức vật liệu" sheetId="2" r:id="rId2"/>
+    <sheet name="Định mức nhân công" sheetId="3" r:id="rId3"/>
+    <sheet name="Định mức máy" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -470,6 +473,18 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,18 +499,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +821,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -837,143 +840,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="str">
+      <c r="B2" s="39" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="str">
+      <c r="B3" s="39" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
     </row>
     <row r="4" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="36" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33" t="s">
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33" t="s">
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
       <c r="Y4" s="17"/>
     </row>
     <row r="5" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
       <c r="F5" s="20" t="s">
         <v>10</v>
       </c>
@@ -992,8 +995,8 @@
       <c r="K5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="20" t="s">
         <v>16</v>
       </c>
@@ -1320,25 +1323,25 @@
       <c r="AA15" s="7"/>
     </row>
     <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="35"/>
       <c r="R16" s="21">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
@@ -1371,13 +1374,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A16:Q16"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="B1:X1"/>
@@ -1386,6 +1382,13 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="B3:X3"/>
+    <mergeCell ref="A16:Q16"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="V6 V10:V17">
     <cfRule type="cellIs" dxfId="5" priority="16" stopIfTrue="1" operator="equal">
@@ -1420,4 +1423,61 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" customWidth="1"/>
+    <col min="4" max="8" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
+    <col min="4" max="7" width="15.44140625" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="7" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hiển thị định mức vật liệu, nhân công, máy
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -821,7 +821,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1430,7 +1430,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K24"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1438,6 +1438,9 @@
     <col min="2" max="2" width="10.21875" customWidth="1"/>
     <col min="3" max="3" width="40.21875" customWidth="1"/>
     <col min="4" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="30.44140625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1449,14 +1452,16 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1048576"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.77734375" customWidth="1"/>
     <col min="3" max="3" width="37.44140625" customWidth="1"/>
-    <col min="4" max="7" width="15.44140625" customWidth="1"/>
+    <col min="4" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="36.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1468,14 +1473,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="39.44140625" customWidth="1"/>
-    <col min="4" max="7" width="17.44140625" customWidth="1"/>
+    <col min="4" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sử dụng chung template
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -13,9 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Tiên lượng" sheetId="1" r:id="rId1"/>
-    <sheet name="Định mức vật liệu" sheetId="2" r:id="rId2"/>
-    <sheet name="Định mức nhân công" sheetId="3" r:id="rId3"/>
-    <sheet name="Định mức máy" sheetId="4" r:id="rId4"/>
+    <sheet name="Giá vật liệu" sheetId="5" r:id="rId2"/>
+    <sheet name="Cước ô tô" sheetId="6" r:id="rId3"/>
+    <sheet name="Cước biển" sheetId="7" r:id="rId4"/>
+    <sheet name="Cước TC" sheetId="8" r:id="rId5"/>
+    <sheet name="Cước sông" sheetId="9" r:id="rId6"/>
+    <sheet name="Định mức vật liệu" sheetId="2" r:id="rId7"/>
+    <sheet name="Định mức nhân công" sheetId="3" r:id="rId8"/>
+    <sheet name="Định mức máy" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>BẢNG DỰ TOÁN HẠNG MỤC CÔNG TRÌNH</t>
   </si>
@@ -105,17 +110,75 @@
   </si>
   <si>
     <t>Ký hiệu bản vẽ</t>
+  </si>
+  <si>
+    <t>BẢNG GIÁ VẬT LIỆU</t>
+  </si>
+  <si>
+    <t>Theo Công bố số …/2023/CBGVL-Ls ngày …/…/2023 của Liên Sở Xây dựng - Tài chính</t>
+  </si>
+  <si>
+    <t>Đơn vị tính: Đồng</t>
+  </si>
+  <si>
+    <t>Mã hiệu</t>
+  </si>
+  <si>
+    <t>Tên vật liệu</t>
+  </si>
+  <si>
+    <t>Giá gốc</t>
+  </si>
+  <si>
+    <t>Giá TB</t>
+  </si>
+  <si>
+    <t>Hệ số</t>
+  </si>
+  <si>
+    <t>Giá TB x HS</t>
+  </si>
+  <si>
+    <t>Cước ô tô</t>
+  </si>
+  <si>
+    <t>Cước ô tô mới</t>
+  </si>
+  <si>
+    <t>Cước sông</t>
+  </si>
+  <si>
+    <t>Cước TC</t>
+  </si>
+  <si>
+    <t>Cước nội bộ</t>
+  </si>
+  <si>
+    <t>Cước biển</t>
+  </si>
+  <si>
+    <t>Cước khác</t>
+  </si>
+  <si>
+    <t>Tổng cước</t>
+  </si>
+  <si>
+    <t>Giá HT</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="###,###,##0.0000"/>
     <numFmt numFmtId="165" formatCode="###,###,###,##0"/>
+    <numFmt numFmtId="166" formatCode="###,###,###.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +241,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10.5"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -205,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -379,11 +466,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -473,6 +573,21 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -485,26 +600,53 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -821,7 +963,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -840,143 +982,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="str">
+      <c r="B2" s="35" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="str">
+      <c r="B3" s="35" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
     </row>
     <row r="4" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="40" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37" t="s">
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37" t="s">
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
       <c r="Y4" s="17"/>
     </row>
     <row r="5" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="20" t="s">
         <v>10</v>
       </c>
@@ -995,8 +1137,8 @@
       <c r="K5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
       <c r="N5" s="20" t="s">
         <v>16</v>
       </c>
@@ -1323,25 +1465,25 @@
       <c r="AA15" s="7"/>
     </row>
     <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="35"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="40"/>
       <c r="R16" s="21">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
@@ -1374,6 +1516,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A16:Q16"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="R4:U4"/>
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="B1:X1"/>
@@ -1382,41 +1531,34 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="B3:X3"/>
-    <mergeCell ref="A16:Q16"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="V6 V10:V17">
-    <cfRule type="cellIs" dxfId="5" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W6 W10:W17">
-    <cfRule type="cellIs" dxfId="4" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="17" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6 X10:X17">
-    <cfRule type="cellIs" dxfId="3" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="18" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7:V9">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7:W9">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7:X9">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1426,6 +1568,495 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:W15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="21" width="18" customWidth="1"/>
+    <col min="22" max="22" width="16.21875" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B1" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q4" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="U4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="W4" s="45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+    </row>
+    <row r="6" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="47"/>
+    </row>
+    <row r="7" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+    </row>
+    <row r="8" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+    </row>
+    <row r="9" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+    </row>
+    <row r="10" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+    </row>
+    <row r="11" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+    </row>
+    <row r="12" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="47"/>
+    </row>
+    <row r="13" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+    </row>
+    <row r="14" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="52"/>
+      <c r="T14" s="52"/>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="51"/>
+    </row>
+    <row r="15" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="B3:V3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="K14:K15">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1447,7 +2078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1468,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
đổi sang sử dụng Spreadsheet syncfusion
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -230,12 +230,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11.25"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <name val="Times New Roman"/>
@@ -262,6 +256,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11.25"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -483,12 +483,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -502,9 +499,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -555,9 +549,6 @@
     <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -572,42 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -627,7 +582,7 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,8 +590,47 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,7 +957,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -977,542 +971,542 @@
     <col min="12" max="13" width="13.5546875" style="1" customWidth="1"/>
     <col min="14" max="21" width="13.33203125" style="1" customWidth="1"/>
     <col min="22" max="24" width="7.6640625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="132.109375" style="18" customWidth="1"/>
+    <col min="25" max="25" width="132.109375" style="16" customWidth="1"/>
     <col min="26" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="str">
+      <c r="B2" s="48" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="str">
+      <c r="B3" s="48" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-    </row>
-    <row r="4" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+    </row>
+    <row r="4" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="36" t="s">
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33" t="s">
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33" t="s">
+      <c r="S4" s="46"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="17"/>
-    </row>
-    <row r="5" spans="1:27" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="20" t="s">
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="54"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="20" t="s">
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="R5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="T5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="20" t="s">
+      <c r="U5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="20" t="s">
+      <c r="V5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="W5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="20" t="s">
+      <c r="X5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="Y5" s="17"/>
+      <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="7"/>
-      <c r="AA9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="29"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="32"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="30"/>
-      <c r="W12" s="30"/>
-      <c r="X12" s="30"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
     </row>
     <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="7"/>
-      <c r="AA13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="58"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
     </row>
     <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="58"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
     </row>
     <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="21">
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="19">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="21">
+      <c r="S16" s="19">
         <f>SUMIF(B6:B15,"&gt;0",S6:S15)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="21">
+      <c r="T16" s="19">
         <f>SUMIF(B6:B15,"&gt;0",T6:T15)</f>
         <v>0</v>
       </c>
-      <c r="U16" s="21">
+      <c r="U16" s="19">
         <f>SUMIF(B6:B15,"&gt;0",U6:U15)</f>
         <v>0</v>
       </c>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
     </row>
     <row r="17" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1590,406 +1584,406 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
       <c r="W2" s="1"/>
     </row>
     <row r="3" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="2:23" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="Q4" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45" t="s">
+      <c r="R4" s="30"/>
+      <c r="S4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="45" t="s">
+      <c r="T4" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="45" t="s">
+      <c r="U4" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="45" t="s">
+      <c r="V4" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="45" t="s">
+      <c r="W4" s="30" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
     </row>
     <row r="6" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="47"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="47"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
     </row>
     <row r="7" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-      <c r="S7" s="47"/>
-      <c r="T7" s="47"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="47"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
     </row>
     <row r="8" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="47"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
     </row>
     <row r="9" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
     </row>
     <row r="10" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="47"/>
-      <c r="V10" s="47"/>
-      <c r="W10" s="47"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
     </row>
     <row r="11" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
     </row>
     <row r="12" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="47"/>
-      <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="47"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
     </row>
     <row r="13" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
     </row>
     <row r="14" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="49"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="51"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="36"/>
     </row>
     <row r="15" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="57"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
bind và render cho giá vật liệu theo ppt
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -178,7 +178,7 @@
     <numFmt numFmtId="165" formatCode="###,###,###,##0"/>
     <numFmt numFmtId="166" formatCode="###,###,###.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,12 +254,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="11.25"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -483,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,31 +561,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -627,9 +622,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -957,7 +949,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B1" sqref="B1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -976,143 +968,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="48" t="str">
+      <c r="B2" s="47" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="str">
+      <c r="B3" s="47" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
     </row>
     <row r="4" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="49" t="s">
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="49" t="s">
+      <c r="M4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="46" t="s">
+      <c r="N4" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46" t="s">
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46" t="s">
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="46"/>
-      <c r="X4" s="46"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
       <c r="Y4" s="15"/>
     </row>
     <row r="5" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="18" t="s">
         <v>10</v>
       </c>
@@ -1131,8 +1123,8 @@
       <c r="K5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
       <c r="N5" s="18" t="s">
         <v>16</v>
       </c>
@@ -1181,7 +1173,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="20"/>
-      <c r="M6" s="58"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -1210,7 +1202,7 @@
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="58"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -1239,7 +1231,7 @@
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="58"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
@@ -1268,7 +1260,7 @@
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="58"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
@@ -1297,7 +1289,7 @@
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="58"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
@@ -1326,7 +1318,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="58"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -1355,7 +1347,7 @@
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="58"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
@@ -1384,7 +1376,7 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="21"/>
-      <c r="M13" s="58"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
@@ -1413,7 +1405,7 @@
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="58"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
@@ -1442,7 +1434,7 @@
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
       <c r="L15" s="21"/>
-      <c r="M15" s="58"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
@@ -1459,25 +1451,25 @@
       <c r="AA15" s="6"/>
     </row>
     <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="52"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="53"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="52"/>
       <c r="R16" s="19">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
@@ -1566,7 +1558,7 @@
   <dimension ref="B1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1584,81 +1576,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
       <c r="W1" s="1"/>
     </row>
     <row r="2" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
       <c r="W2" s="1"/>
     </row>
     <row r="3" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="2:23" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1722,244 +1714,244 @@
       </c>
     </row>
     <row r="5" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
     </row>
     <row r="6" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="33"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
     </row>
     <row r="7" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="33"/>
+      <c r="T7" s="33"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
     </row>
     <row r="8" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-      <c r="T8" s="32"/>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
     </row>
     <row r="9" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
     </row>
     <row r="10" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-      <c r="T10" s="32"/>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
     </row>
     <row r="11" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-      <c r="T11" s="32"/>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="33"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="33"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
     </row>
     <row r="12" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="33"/>
+      <c r="T12" s="33"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
     </row>
     <row r="13" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="33"/>
-      <c r="T13" s="33"/>
-      <c r="U13" s="33"/>
-      <c r="V13" s="33"/>
-      <c r="W13" s="33"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
     </row>
     <row r="14" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="38"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="36"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="38"/>
+      <c r="V14" s="38"/>
+      <c r="W14" s="37"/>
     </row>
     <row r="15" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="40"/>
@@ -1970,8 +1962,8 @@
       <c r="G15" s="43"/>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="45"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
       <c r="L15" s="43"/>
       <c r="M15" s="43"/>
       <c r="N15" s="43"/>
@@ -1997,6 +1989,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
thêm hook insert và delete vào tiên lượng
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/TienLuong.xlsx
+++ b/Worksheet/Content/Template/TienLuong.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\dev\c-sharp-patterns\Worksheet\Content\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\c-sharp-patterns\Worksheet\Content\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -280,7 +280,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -339,36 +339,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
@@ -471,123 +441,147 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -942,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:X1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -957,542 +951,542 @@
     <col min="12" max="13" width="13.5546875" style="1" customWidth="1"/>
     <col min="14" max="21" width="13.33203125" style="1" customWidth="1"/>
     <col min="22" max="24" width="7.6640625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="132.109375" style="16" customWidth="1"/>
+    <col min="25" max="25" width="132.109375" style="6" customWidth="1"/>
     <col min="26" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
     </row>
     <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="51" t="str">
+      <c r="B2" s="59" t="str">
         <f>"CÔNG TRÌNH: " &amp;"Công trình 1"</f>
         <v>CÔNG TRÌNH: Công trình 1</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="str">
+      <c r="B3" s="59" t="str">
         <f>"HẠNG MỤC: " &amp;"Hạng mục 1"</f>
         <v>HẠNG MỤC: Hạng mục 1</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-    </row>
-    <row r="4" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+    </row>
+    <row r="4" spans="1:27" s="7" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="52" t="s">
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="52" t="s">
+      <c r="M4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49" t="s">
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49" t="s">
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:27" s="17" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="18" t="s">
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="5"/>
+    </row>
+    <row r="5" spans="1:27" s="7" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="56"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="18" t="s">
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="18" t="s">
+      <c r="R5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="18" t="s">
+      <c r="S5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="T5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="18" t="s">
+      <c r="V5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="W5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y5" s="15"/>
+      <c r="Y5" s="5"/>
     </row>
     <row r="6" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="29"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="23"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="29"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="29"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="45"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="29"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="44"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="23"/>
-      <c r="S13" s="23"/>
-      <c r="T13" s="23"/>
-      <c r="U13" s="23"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="29"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="44"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="23"/>
-      <c r="V14" s="27"/>
-      <c r="W14" s="27"/>
-      <c r="X14" s="27"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="28"/>
-      <c r="Y15" s="29"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="19">
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="54"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="9">
         <f>SUMIF(B6:B15,"&gt;0",R6:R15)</f>
         <v>0</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="9">
         <f>SUMIF(B6:B15,"&gt;0",S6:S15)</f>
         <v>0</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="9">
         <f>SUMIF(B6:B15,"&gt;0",T6:T15)</f>
         <v>0</v>
       </c>
-      <c r="U16" s="19">
+      <c r="U16" s="9">
         <f>SUMIF(B6:B15,"&gt;0",U6:U15)</f>
         <v>0</v>
       </c>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
     </row>
     <row r="17" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1568,312 +1562,312 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="30" t="s">
+      <c r="H4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="K4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="O4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
     </row>
     <row r="7" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
     </row>
     <row r="8" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
     </row>
     <row r="9" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
     </row>
     <row r="10" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="33"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
     </row>
     <row r="11" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
     </row>
     <row r="12" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
     </row>
     <row r="13" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
     </row>
     <row r="14" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="37"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="43"/>
-      <c r="N15" s="43"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="42"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>